<commit_message>
Network training  and evaluation updated with 100 epochsd
Even though in the 5 models some only reached 25 epochs before passing to the next
</commit_message>
<xml_diff>
--- a/Project/code/intermediate/models/transformers_only_training_runs.xlsx
+++ b/Project/code/intermediate/models/transformers_only_training_runs.xlsx
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J2" t="n">
         <v>32</v>
@@ -723,16 +723,16 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>05/20/2024 23:27:10</t>
+          <t>05/22/2024 00:51:42</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>05/21/2024 00:04:40</t>
+          <t>05/22/2024 02:42:14</t>
         </is>
       </c>
       <c r="AH2" t="n">
-        <v>0.3998939620514166</v>
+        <v>0.3866017184072858</v>
       </c>
     </row>
     <row r="3">
@@ -769,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J3" t="n">
         <v>32</v>
@@ -853,16 +853,16 @@
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>05/21/2024 00:04:40</t>
+          <t>05/22/2024 02:42:15</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>05/21/2024 00:42:33</t>
+          <t>05/22/2024 04:34:42</t>
         </is>
       </c>
       <c r="AH3" t="n">
-        <v>0.4230562371354928</v>
+        <v>0.3744101685495928</v>
       </c>
     </row>
     <row r="4">
@@ -899,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J4" t="n">
         <v>32</v>
@@ -983,16 +983,16 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>05/21/2024 00:42:33</t>
+          <t>05/22/2024 04:34:42</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>05/21/2024 01:22:05</t>
+          <t>05/22/2024 06:44:40</t>
         </is>
       </c>
       <c r="AH4" t="n">
-        <v>0.4059906424707799</v>
+        <v>0.3931281571844637</v>
       </c>
     </row>
     <row r="5">
@@ -1029,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J5" t="n">
         <v>32</v>
@@ -1113,16 +1113,16 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>05/21/2024 01:22:05</t>
+          <t>05/22/2024 06:44:40</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>05/21/2024 02:02:56</t>
+          <t>05/22/2024 08:19:29</t>
         </is>
       </c>
       <c r="AH5" t="n">
-        <v>0.4547020230945617</v>
+        <v>0.4401574363816773</v>
       </c>
     </row>
     <row r="6">
@@ -1159,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="J6" t="n">
         <v>32</v>
@@ -1243,16 +1243,16 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>05/21/2024 02:02:57</t>
+          <t>05/22/2024 08:19:30</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>05/21/2024 02:43:05</t>
+          <t>05/22/2024 10:11:48</t>
         </is>
       </c>
       <c r="AH6" t="n">
-        <v>0.4564282326261911</v>
+        <v>0.4253510647461318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start new network training with all vision transformer models/variants
</commit_message>
<xml_diff>
--- a/Project/code/intermediate/models/transformers_only_training_runs.xlsx
+++ b/Project/code/intermediate/models/transformers_only_training_runs.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Universidade de Lisboa\FCUL\2 Semestre\AP\fcul-deep-learning\Project\code\intermediate\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B7469-AA82-4D61-963C-DCB99C927D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE91513-19FF-40E3-A1CE-63DA9C1CCD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21480" yWindow="0" windowWidth="21600" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -149,13 +162,22 @@
   </si>
   <si>
     <t>adam</t>
+  </si>
+  <si>
+    <t>Swin</t>
+  </si>
+  <si>
+    <t>DeiT</t>
+  </si>
+  <si>
+    <t>CaiT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +189,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AD14" sqref="AD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,6 +748,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>SUM(A2+1)</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -738,6 +767,7 @@
         <v>37</v>
       </c>
       <c r="G3">
+        <f>SUM(G2+1)</f>
         <v>2</v>
       </c>
       <c r="H3">
@@ -815,6 +845,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A21" si="0">SUM(A3+1)</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -833,6 +864,7 @@
         <v>37</v>
       </c>
       <c r="G4">
+        <f t="shared" ref="G4:G21" si="1">SUM(G3+1)</f>
         <v>3</v>
       </c>
       <c r="H4">
@@ -910,6 +942,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -928,6 +961,7 @@
         <v>37</v>
       </c>
       <c r="G5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H5">
@@ -1005,6 +1039,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1023,6 +1058,7 @@
         <v>37</v>
       </c>
       <c r="G6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H6">
@@ -1098,7 +1134,1463 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>32</v>
+      </c>
+      <c r="K7">
+        <v>16</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" t="b">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC7">
+        <v>5</v>
+      </c>
+      <c r="AD7">
+        <v>0.5</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>32</v>
+      </c>
+      <c r="K8">
+        <v>16</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" t="s">
+        <v>40</v>
+      </c>
+      <c r="U8" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" t="b">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB8">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC8">
+        <v>5</v>
+      </c>
+      <c r="AD8">
+        <v>0.5</v>
+      </c>
+      <c r="AE8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
+        <v>32</v>
+      </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9" t="s">
+        <v>40</v>
+      </c>
+      <c r="U9" t="s">
+        <v>40</v>
+      </c>
+      <c r="V9" t="b">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB9">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC9">
+        <v>5</v>
+      </c>
+      <c r="AD9">
+        <v>0.5</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
+      <c r="S10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V10" t="b">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB10">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC10">
+        <v>5</v>
+      </c>
+      <c r="AD10">
+        <v>0.5</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>32</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11" t="s">
+        <v>39</v>
+      </c>
+      <c r="T11" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB11">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC11">
+        <v>5</v>
+      </c>
+      <c r="AD11">
+        <v>0.5</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <v>32</v>
+      </c>
+      <c r="K12">
+        <v>16</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12" t="s">
+        <v>39</v>
+      </c>
+      <c r="T12" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB12">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC12">
+        <v>5</v>
+      </c>
+      <c r="AD12">
+        <v>0.5</v>
+      </c>
+      <c r="AE12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
+      <c r="J13">
+        <v>32</v>
+      </c>
+      <c r="K13">
+        <v>16</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
+      <c r="S13" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13" t="s">
+        <v>40</v>
+      </c>
+      <c r="U13" t="s">
+        <v>40</v>
+      </c>
+      <c r="V13" t="b">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB13">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC13">
+        <v>5</v>
+      </c>
+      <c r="AD13">
+        <v>0.5</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>32</v>
+      </c>
+      <c r="K14">
+        <v>16</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="O14" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14" t="s">
+        <v>39</v>
+      </c>
+      <c r="T14" t="s">
+        <v>40</v>
+      </c>
+      <c r="U14" t="s">
+        <v>40</v>
+      </c>
+      <c r="V14" t="b">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB14">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC14">
+        <v>5</v>
+      </c>
+      <c r="AD14">
+        <v>0.5</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15">
+        <v>32</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+      <c r="O15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T15" t="s">
+        <v>40</v>
+      </c>
+      <c r="U15" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" t="b">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB15">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC15">
+        <v>5</v>
+      </c>
+      <c r="AD15">
+        <v>0.5</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>100</v>
+      </c>
+      <c r="J16">
+        <v>32</v>
+      </c>
+      <c r="K16">
+        <v>16</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>3</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="S16" t="s">
+        <v>39</v>
+      </c>
+      <c r="T16" t="s">
+        <v>40</v>
+      </c>
+      <c r="U16" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" t="b">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB16">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC16">
+        <v>5</v>
+      </c>
+      <c r="AD16">
+        <v>0.5</v>
+      </c>
+      <c r="AE16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>32</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>10</v>
+      </c>
+      <c r="O17" t="s">
+        <v>45</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>3</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="S17" t="s">
+        <v>39</v>
+      </c>
+      <c r="T17" t="s">
+        <v>40</v>
+      </c>
+      <c r="U17" t="s">
+        <v>40</v>
+      </c>
+      <c r="V17" t="b">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB17">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC17">
+        <v>5</v>
+      </c>
+      <c r="AD17">
+        <v>0.5</v>
+      </c>
+      <c r="AE17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>100</v>
+      </c>
+      <c r="J18">
+        <v>32</v>
+      </c>
+      <c r="K18">
+        <v>16</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>10</v>
+      </c>
+      <c r="O18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>2</v>
+      </c>
+      <c r="S18" t="s">
+        <v>39</v>
+      </c>
+      <c r="T18" t="s">
+        <v>40</v>
+      </c>
+      <c r="U18" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" t="b">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB18">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC18">
+        <v>5</v>
+      </c>
+      <c r="AD18">
+        <v>0.5</v>
+      </c>
+      <c r="AE18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>32</v>
+      </c>
+      <c r="K19">
+        <v>16</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>3</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="S19" t="s">
+        <v>39</v>
+      </c>
+      <c r="T19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U19" t="s">
+        <v>40</v>
+      </c>
+      <c r="V19" t="b">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB19">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC19">
+        <v>5</v>
+      </c>
+      <c r="AD19">
+        <v>0.5</v>
+      </c>
+      <c r="AE19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>100</v>
+      </c>
+      <c r="J20">
+        <v>32</v>
+      </c>
+      <c r="K20">
+        <v>16</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>10</v>
+      </c>
+      <c r="O20" t="s">
+        <v>45</v>
+      </c>
+      <c r="P20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20" t="s">
+        <v>39</v>
+      </c>
+      <c r="T20" t="s">
+        <v>40</v>
+      </c>
+      <c r="U20" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20" t="b">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB20">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC20">
+        <v>5</v>
+      </c>
+      <c r="AD20">
+        <v>0.5</v>
+      </c>
+      <c r="AE20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>32</v>
+      </c>
+      <c r="K21">
+        <v>16</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>10</v>
+      </c>
+      <c r="O21" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>3</v>
+      </c>
+      <c r="R21">
+        <v>2</v>
+      </c>
+      <c r="S21" t="s">
+        <v>39</v>
+      </c>
+      <c r="T21" t="s">
+        <v>40</v>
+      </c>
+      <c r="U21" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" t="b">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB21">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="AC21">
+        <v>5</v>
+      </c>
+      <c r="AD21">
+        <v>0.5</v>
+      </c>
+      <c r="AE21" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>